<commit_message>
Five wave files performance evaluation done
</commit_message>
<xml_diff>
--- a/Evaluation Code/Reference/MasterList.xlsx
+++ b/Evaluation Code/Reference/MasterList.xlsx
@@ -164,409 +164,413 @@
     <t>ClaraBerryAndWooldog_Stella</t>
   </si>
   <si>
+    <t>[ 05 ]</t>
+  </si>
+  <si>
+    <t>[ 01;02;03;04 ]</t>
+  </si>
+  <si>
+    <t>[ 01;07;08;09 ]</t>
+  </si>
+  <si>
+    <t>[ 02;03;04;05;06;10 ]</t>
+  </si>
+  <si>
+    <t>DreamersOfTheGhetto_HeavyLove</t>
+  </si>
+  <si>
+    <t>Pop</t>
+  </si>
+  <si>
+    <t>[ 02;06;08 ]</t>
+  </si>
+  <si>
+    <t>[ 01;03;04;05;07;09 ]</t>
+  </si>
+  <si>
+    <t>FacesOnFilm_WaitingForGa</t>
+  </si>
+  <si>
+    <t>[ 03;09;10 ]</t>
+  </si>
+  <si>
+    <t>[ 01;02;04;05;06;07;08;11 ]</t>
+  </si>
+  <si>
+    <t>Grants_PunchDrunk</t>
+  </si>
+  <si>
+    <t>Rap</t>
+  </si>
+  <si>
+    <t>[ 03;04;07 ]</t>
+  </si>
+  <si>
+    <t>[ 01;02;05;06;08;09;10 ]</t>
+  </si>
+  <si>
+    <t>HeladoNegro_MitadDelMundo</t>
+  </si>
+  <si>
+    <t>HezekiahJones_BorrowedHeart</t>
+  </si>
+  <si>
+    <t>[ 02;06;10 ]</t>
+  </si>
+  <si>
+    <t>[ 01;03;04;05;07;08;09;11;12 ]</t>
+  </si>
+  <si>
+    <t>HopAlong_SisterCities</t>
+  </si>
+  <si>
+    <t>[ 03;07 ]</t>
+  </si>
+  <si>
+    <t>[ 01;02;04;05;06;08 ]</t>
+  </si>
+  <si>
+    <t>InvisibleFamiliars_DisturbingWildlife</t>
+  </si>
+  <si>
+    <t>[ 07;08;09 ]</t>
+  </si>
+  <si>
+    <t>[ 01;02;03;04;05;06;10 ]</t>
+  </si>
+  <si>
+    <t>LizNelson_Coldwar</t>
+  </si>
+  <si>
+    <t>LizNelson_Rainfall</t>
+  </si>
+  <si>
+    <t>[ 01;02;03 ]</t>
+  </si>
+  <si>
+    <t>Lushlife_ToynbeeSuite</t>
+  </si>
+  <si>
+    <t>[ 17;18;26 ]</t>
+  </si>
+  <si>
+    <t>[ 01;02;03;04;05;06;07;08;09;10;11;12;13;14;15;16;19;20;21;22;23;24;25 ]</t>
+  </si>
+  <si>
+    <t>MatthewEntwistle_DontYouEver</t>
+  </si>
+  <si>
+    <t>Jazz</t>
+  </si>
+  <si>
+    <t>[ 07 ]</t>
+  </si>
+  <si>
+    <t>Meaxic_TakeAStep</t>
+  </si>
+  <si>
+    <t>[ 04;06;07;08 ]</t>
+  </si>
+  <si>
+    <t>[ 01;02;03;05 ]</t>
+  </si>
+  <si>
+    <t>Meaxic_YouListen</t>
+  </si>
+  <si>
+    <t>[ 03;04;05;06;07 ]</t>
+  </si>
+  <si>
+    <t>MusicDelta_80sRock</t>
+  </si>
+  <si>
+    <t>[ 04 ]</t>
+  </si>
+  <si>
+    <t>MusicDelta_Beatles</t>
+  </si>
+  <si>
+    <t>MusicDelta_Britpop</t>
+  </si>
+  <si>
+    <t>MusicDelta_Country2</t>
+  </si>
+  <si>
+    <t>MusicDelta_Gospel</t>
+  </si>
+  <si>
+    <t>[ 01;02;03;04;05 ]</t>
+  </si>
+  <si>
+    <t>MusicDelta_Grunge</t>
+  </si>
+  <si>
+    <t>MusicDelta_Hendrix</t>
+  </si>
+  <si>
+    <t>MusicDelta_Punk</t>
+  </si>
+  <si>
+    <t>MusicDelta_Reggae</t>
+  </si>
+  <si>
+    <t>MusicDelta_Rock</t>
+  </si>
+  <si>
+    <t>MusicDelta_Rockabilly</t>
+  </si>
+  <si>
+    <t>NightPanther_Fire</t>
+  </si>
+  <si>
+    <t>[ 02;03;07 ]</t>
+  </si>
+  <si>
+    <t>[ 01;04;05;06;08;09;10;11;12 ]</t>
+  </si>
+  <si>
+    <t>PortStWillow_StayEven</t>
+  </si>
+  <si>
+    <t>[ 01;08 ]</t>
+  </si>
+  <si>
+    <t>[ 02;03;04;05;06;07;09;10;11 ]</t>
+  </si>
+  <si>
+    <t>SecretMountains_HighHorse</t>
+  </si>
+  <si>
+    <t>[ 02;09 ]</t>
+  </si>
+  <si>
+    <t>[ 01;03;04;05;06;07;08;10 ]</t>
+  </si>
+  <si>
+    <t>Snowmine_Curfews</t>
+  </si>
+  <si>
+    <t>[ 03;10 ]</t>
+  </si>
+  <si>
+    <t>[ 01;02;04;05;06;07;08;09;11 ]</t>
+  </si>
+  <si>
+    <t>StevenClark_Bounty</t>
+  </si>
+  <si>
+    <t>[ 03;07;08 ]</t>
+  </si>
+  <si>
+    <t>[ 01;02;04;05;06;09;10 ]</t>
+  </si>
+  <si>
+    <t>StrandOfOaks_Spacestation</t>
+  </si>
+  <si>
+    <t>[ 02;04 ]</t>
+  </si>
+  <si>
+    <t>[ 01;03;05;06;07;08 ]</t>
+  </si>
+  <si>
+    <t>SweetLights_YouLetMeDown</t>
+  </si>
+  <si>
+    <t>[ 01;02;04;05;06;07;09;10;11;12;13 ]</t>
+  </si>
+  <si>
+    <t>TheDistricts_Vermont</t>
+  </si>
+  <si>
+    <t>[ 02;05 ]</t>
+  </si>
+  <si>
+    <t>[ 01;03;04;06;07 ]</t>
+  </si>
+  <si>
+    <t>TheScarletBrand_LesFleursDuMal</t>
+  </si>
+  <si>
+    <t>[ 08 ]</t>
+  </si>
+  <si>
+    <t>[ 01;02;03;04;05;06;07 ]</t>
+  </si>
+  <si>
+    <t>TheSoSoGlos_Emergency</t>
+  </si>
+  <si>
+    <t>[ 01;03;04;06;07;08;09;10 ]</t>
+  </si>
+  <si>
+    <t>Excerpt_01</t>
+  </si>
+  <si>
+    <t>Excerpt_02</t>
+  </si>
+  <si>
+    <t>Excerpt_03</t>
+  </si>
+  <si>
+    <t>Excerpt_04</t>
+  </si>
+  <si>
+    <t>Excerpt_05</t>
+  </si>
+  <si>
+    <t>Excerpt_06</t>
+  </si>
+  <si>
+    <t>Excerpt_07</t>
+  </si>
+  <si>
+    <t>Excerpt_08</t>
+  </si>
+  <si>
+    <t>Excerpt_09</t>
+  </si>
+  <si>
+    <t>Excerpt_10</t>
+  </si>
+  <si>
+    <t>Excerpt_11</t>
+  </si>
+  <si>
+    <t>Excerpt_12</t>
+  </si>
+  <si>
+    <t>Excerpt_13</t>
+  </si>
+  <si>
+    <t>Excerpt_14</t>
+  </si>
+  <si>
+    <t>Excerpt_15</t>
+  </si>
+  <si>
+    <t>Excerpt_16</t>
+  </si>
+  <si>
+    <t>Excerpt_17</t>
+  </si>
+  <si>
+    <t>Excerpt_18</t>
+  </si>
+  <si>
+    <t>Excerpt_19</t>
+  </si>
+  <si>
+    <t>Excerpt_20</t>
+  </si>
+  <si>
+    <t>Excerpt_21</t>
+  </si>
+  <si>
+    <t>Excerpt_22</t>
+  </si>
+  <si>
+    <t>Excerpt_23</t>
+  </si>
+  <si>
+    <t>Excerpt_24</t>
+  </si>
+  <si>
+    <t>Excerpt_25</t>
+  </si>
+  <si>
+    <t>Excerpt_26</t>
+  </si>
+  <si>
+    <t>Excerpt_27</t>
+  </si>
+  <si>
+    <t>Excerpt_28</t>
+  </si>
+  <si>
+    <t>Excerpt_29</t>
+  </si>
+  <si>
+    <t>Excerpt_30</t>
+  </si>
+  <si>
+    <t>Excerpt_31</t>
+  </si>
+  <si>
+    <t>Excerpt_32</t>
+  </si>
+  <si>
+    <t>Excerpt_33</t>
+  </si>
+  <si>
+    <t>Excerpt_34</t>
+  </si>
+  <si>
+    <t>Excerpt_35</t>
+  </si>
+  <si>
+    <t>Excerpt_36</t>
+  </si>
+  <si>
+    <t>Excerpt_37</t>
+  </si>
+  <si>
+    <t>Excerpt_38</t>
+  </si>
+  <si>
+    <t>Excerpt_39</t>
+  </si>
+  <si>
+    <t>Excerpt_40</t>
+  </si>
+  <si>
+    <t>Excerpt_41</t>
+  </si>
+  <si>
+    <t>Excerpt_42</t>
+  </si>
+  <si>
+    <t>Excerpt_43</t>
+  </si>
+  <si>
+    <t>Excerpt_44</t>
+  </si>
+  <si>
+    <t>Excerpt_45</t>
+  </si>
+  <si>
+    <t>Excerpt_46</t>
+  </si>
+  <si>
+    <t>Excerpt_47</t>
+  </si>
+  <si>
+    <t>Excerpt_48</t>
+  </si>
+  <si>
+    <t>Excerpt_49</t>
+  </si>
+  <si>
+    <t>Excerpt_50</t>
+  </si>
+  <si>
+    <t>Excerpt_51</t>
+  </si>
+  <si>
+    <t>Creepoid_OldTree</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>ClaraBerryAndWooldog_WaltzForMyVictims</t>
-  </si>
-  <si>
-    <t>[ 05 ]</t>
-  </si>
-  <si>
-    <t>[ 01;02;03;04 ]</t>
-  </si>
-  <si>
-    <t>Creepoid_OldTree</t>
-  </si>
-  <si>
-    <t>[ 01;07;08;09 ]</t>
-  </si>
-  <si>
-    <t>[ 02;03;04;05;06;10 ]</t>
-  </si>
-  <si>
-    <t>DreamersOfTheGhetto_HeavyLove</t>
-  </si>
-  <si>
-    <t>Pop</t>
-  </si>
-  <si>
-    <t>[ 02;06;08 ]</t>
-  </si>
-  <si>
-    <t>[ 01;03;04;05;07;09 ]</t>
-  </si>
-  <si>
-    <t>FacesOnFilm_WaitingForGa</t>
-  </si>
-  <si>
-    <t>[ 03;09;10 ]</t>
-  </si>
-  <si>
-    <t>[ 01;02;04;05;06;07;08;11 ]</t>
-  </si>
-  <si>
-    <t>Grants_PunchDrunk</t>
-  </si>
-  <si>
-    <t>Rap</t>
-  </si>
-  <si>
-    <t>[ 03;04;07 ]</t>
-  </si>
-  <si>
-    <t>[ 01;02;05;06;08;09;10 ]</t>
-  </si>
-  <si>
-    <t>HeladoNegro_MitadDelMundo</t>
-  </si>
-  <si>
-    <t>HezekiahJones_BorrowedHeart</t>
-  </si>
-  <si>
-    <t>[ 02;06;10 ]</t>
-  </si>
-  <si>
-    <t>[ 01;03;04;05;07;08;09;11;12 ]</t>
-  </si>
-  <si>
-    <t>HopAlong_SisterCities</t>
-  </si>
-  <si>
-    <t>[ 03;07 ]</t>
-  </si>
-  <si>
-    <t>[ 01;02;04;05;06;08 ]</t>
-  </si>
-  <si>
-    <t>InvisibleFamiliars_DisturbingWildlife</t>
-  </si>
-  <si>
-    <t>[ 07;08;09 ]</t>
-  </si>
-  <si>
-    <t>[ 01;02;03;04;05;06;10 ]</t>
-  </si>
-  <si>
-    <t>LizNelson_Coldwar</t>
-  </si>
-  <si>
-    <t>LizNelson_Rainfall</t>
-  </si>
-  <si>
-    <t>[ 01;02;03 ]</t>
-  </si>
-  <si>
-    <t>Lushlife_ToynbeeSuite</t>
-  </si>
-  <si>
-    <t>[ 17;18;26 ]</t>
-  </si>
-  <si>
-    <t>[ 01;02;03;04;05;06;07;08;09;10;11;12;13;14;15;16;19;20;21;22;23;24;25 ]</t>
-  </si>
-  <si>
-    <t>MatthewEntwistle_DontYouEver</t>
-  </si>
-  <si>
-    <t>Jazz</t>
-  </si>
-  <si>
-    <t>[ 07 ]</t>
-  </si>
-  <si>
-    <t>Meaxic_TakeAStep</t>
-  </si>
-  <si>
-    <t>[ 04;06;07;08 ]</t>
-  </si>
-  <si>
-    <t>[ 01;02;03;05 ]</t>
-  </si>
-  <si>
-    <t>Meaxic_YouListen</t>
-  </si>
-  <si>
-    <t>[ 03;04;05;06;07 ]</t>
-  </si>
-  <si>
-    <t>MusicDelta_80sRock</t>
-  </si>
-  <si>
-    <t>[ 04 ]</t>
-  </si>
-  <si>
-    <t>MusicDelta_Beatles</t>
-  </si>
-  <si>
-    <t>MusicDelta_Britpop</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>MusicDelta_Country1</t>
-  </si>
-  <si>
-    <t>MusicDelta_Country2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>MusicDelta_Disco</t>
-  </si>
-  <si>
-    <t>MusicDelta_Gospel</t>
-  </si>
-  <si>
-    <t>[ 01;02;03;04;05 ]</t>
-  </si>
-  <si>
-    <t>MusicDelta_Grunge</t>
-  </si>
-  <si>
-    <t>MusicDelta_Hendrix</t>
-  </si>
-  <si>
-    <t>MusicDelta_Punk</t>
-  </si>
-  <si>
-    <t>MusicDelta_Reggae</t>
-  </si>
-  <si>
-    <t>MusicDelta_Rock</t>
-  </si>
-  <si>
-    <t>MusicDelta_Rockabilly</t>
-  </si>
-  <si>
-    <t>NightPanther_Fire</t>
-  </si>
-  <si>
-    <t>[ 02;03;07 ]</t>
-  </si>
-  <si>
-    <t>[ 01;04;05;06;08;09;10;11;12 ]</t>
-  </si>
-  <si>
-    <t>PortStWillow_StayEven</t>
-  </si>
-  <si>
-    <t>[ 01;08 ]</t>
-  </si>
-  <si>
-    <t>[ 02;03;04;05;06;07;09;10;11 ]</t>
-  </si>
-  <si>
-    <t>SecretMountains_HighHorse</t>
-  </si>
-  <si>
-    <t>[ 02;09 ]</t>
-  </si>
-  <si>
-    <t>[ 01;03;04;05;06;07;08;10 ]</t>
-  </si>
-  <si>
-    <t>Snowmine_Curfews</t>
-  </si>
-  <si>
-    <t>[ 03;10 ]</t>
-  </si>
-  <si>
-    <t>[ 01;02;04;05;06;07;08;09;11 ]</t>
-  </si>
-  <si>
-    <t>StevenClark_Bounty</t>
-  </si>
-  <si>
-    <t>[ 03;07;08 ]</t>
-  </si>
-  <si>
-    <t>[ 01;02;04;05;06;09;10 ]</t>
-  </si>
-  <si>
-    <t>StrandOfOaks_Spacestation</t>
-  </si>
-  <si>
-    <t>[ 02;04 ]</t>
-  </si>
-  <si>
-    <t>[ 01;03;05;06;07;08 ]</t>
-  </si>
-  <si>
-    <t>SweetLights_YouLetMeDown</t>
-  </si>
-  <si>
-    <t>[ 01;02;04;05;06;07;09;10;11;12;13 ]</t>
-  </si>
-  <si>
-    <t>TheDistricts_Vermont</t>
-  </si>
-  <si>
-    <t>[ 02;05 ]</t>
-  </si>
-  <si>
-    <t>[ 01;03;04;06;07 ]</t>
-  </si>
-  <si>
-    <t>TheScarletBrand_LesFleursDuMal</t>
-  </si>
-  <si>
-    <t>[ 08 ]</t>
-  </si>
-  <si>
-    <t>[ 01;02;03;04;05;06;07 ]</t>
-  </si>
-  <si>
-    <t>TheSoSoGlos_Emergency</t>
-  </si>
-  <si>
-    <t>[ 01;03;04;06;07;08;09;10 ]</t>
-  </si>
-  <si>
-    <t>Excerpt_01</t>
-  </si>
-  <si>
-    <t>Excerpt_02</t>
-  </si>
-  <si>
-    <t>Excerpt_03</t>
-  </si>
-  <si>
-    <t>Excerpt_04</t>
-  </si>
-  <si>
-    <t>Excerpt_05</t>
-  </si>
-  <si>
-    <t>Excerpt_06</t>
-  </si>
-  <si>
-    <t>Excerpt_07</t>
-  </si>
-  <si>
-    <t>Excerpt_08</t>
-  </si>
-  <si>
-    <t>Excerpt_09</t>
-  </si>
-  <si>
-    <t>Excerpt_10</t>
-  </si>
-  <si>
-    <t>Excerpt_11</t>
-  </si>
-  <si>
-    <t>Excerpt_12</t>
-  </si>
-  <si>
-    <t>Excerpt_13</t>
-  </si>
-  <si>
-    <t>Excerpt_14</t>
-  </si>
-  <si>
-    <t>Excerpt_15</t>
-  </si>
-  <si>
-    <t>Excerpt_16</t>
-  </si>
-  <si>
-    <t>Excerpt_17</t>
-  </si>
-  <si>
-    <t>Excerpt_18</t>
-  </si>
-  <si>
-    <t>Excerpt_19</t>
-  </si>
-  <si>
-    <t>Excerpt_20</t>
-  </si>
-  <si>
-    <t>Excerpt_21</t>
-  </si>
-  <si>
-    <t>Excerpt_22</t>
-  </si>
-  <si>
-    <t>Excerpt_23</t>
-  </si>
-  <si>
-    <t>Excerpt_24</t>
-  </si>
-  <si>
-    <t>Excerpt_25</t>
-  </si>
-  <si>
-    <t>Excerpt_26</t>
-  </si>
-  <si>
-    <t>Excerpt_27</t>
-  </si>
-  <si>
-    <t>Excerpt_28</t>
-  </si>
-  <si>
-    <t>Excerpt_29</t>
-  </si>
-  <si>
-    <t>Excerpt_30</t>
-  </si>
-  <si>
-    <t>Excerpt_31</t>
-  </si>
-  <si>
-    <t>Excerpt_32</t>
-  </si>
-  <si>
-    <t>Excerpt_33</t>
-  </si>
-  <si>
-    <t>Excerpt_34</t>
-  </si>
-  <si>
-    <t>Excerpt_35</t>
-  </si>
-  <si>
-    <t>Excerpt_36</t>
-  </si>
-  <si>
-    <t>Excerpt_37</t>
-  </si>
-  <si>
-    <t>Excerpt_38</t>
-  </si>
-  <si>
-    <t>Excerpt_39</t>
-  </si>
-  <si>
-    <t>Excerpt_40</t>
-  </si>
-  <si>
-    <t>Excerpt_41</t>
-  </si>
-  <si>
-    <t>Excerpt_42</t>
-  </si>
-  <si>
-    <t>Excerpt_43</t>
-  </si>
-  <si>
-    <t>Excerpt_44</t>
-  </si>
-  <si>
-    <t>Excerpt_45</t>
-  </si>
-  <si>
-    <t>Excerpt_46</t>
-  </si>
-  <si>
-    <t>Excerpt_47</t>
-  </si>
-  <si>
-    <t>Excerpt_48</t>
-  </si>
-  <si>
-    <t>Excerpt_49</t>
-  </si>
-  <si>
-    <t>Excerpt_50</t>
-  </si>
-  <si>
-    <t>Excerpt_51</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -925,7 +929,7 @@
   <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -974,7 +978,7 @@
         <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
@@ -994,7 +998,7 @@
         <v>14</v>
       </c>
       <c r="F3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
@@ -1014,7 +1018,7 @@
         <v>17</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
@@ -1034,7 +1038,7 @@
         <v>20</v>
       </c>
       <c r="F5" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
@@ -1054,7 +1058,7 @@
         <v>23</v>
       </c>
       <c r="F6" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
@@ -1074,7 +1078,7 @@
         <v>26</v>
       </c>
       <c r="F7" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.15">
@@ -1094,7 +1098,7 @@
         <v>29</v>
       </c>
       <c r="F8" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.15">
@@ -1114,7 +1118,7 @@
         <v>34</v>
       </c>
       <c r="F9" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.15">
@@ -1134,7 +1138,7 @@
         <v>37</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.15">
@@ -1154,7 +1158,7 @@
         <v>39</v>
       </c>
       <c r="F11" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.15">
@@ -1174,7 +1178,7 @@
         <v>42</v>
       </c>
       <c r="F12" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.15">
@@ -1194,7 +1198,7 @@
         <v>45</v>
       </c>
       <c r="F13" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.15">
@@ -1214,12 +1218,12 @@
         <v>42</v>
       </c>
       <c r="F14" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
-        <v>47</v>
+        <v>179</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>7</v>
@@ -1228,18 +1232,18 @@
         <v>12</v>
       </c>
       <c r="D15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="F15" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>50</v>
+        <v>178</v>
       </c>
       <c r="B16" t="s">
         <v>25</v>
@@ -1248,38 +1252,38 @@
         <v>8</v>
       </c>
       <c r="D16" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E16" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F16" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B17" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C17" t="s">
         <v>32</v>
       </c>
       <c r="D17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E17" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F17" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B18" t="s">
         <v>7</v>
@@ -1288,41 +1292,41 @@
         <v>8</v>
       </c>
       <c r="D18" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E18" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F18" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" t="s">
         <v>60</v>
       </c>
-      <c r="B19" t="s">
+      <c r="E19" t="s">
         <v>61</v>
       </c>
-      <c r="C19" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19" t="s">
-        <v>62</v>
-      </c>
-      <c r="E19" t="s">
-        <v>63</v>
-      </c>
       <c r="F19" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B20" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C20" t="s">
         <v>8</v>
@@ -1334,12 +1338,12 @@
         <v>23</v>
       </c>
       <c r="F20" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B21" t="s">
         <v>7</v>
@@ -1348,18 +1352,18 @@
         <v>8</v>
       </c>
       <c r="D21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F21" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B22" t="s">
         <v>25</v>
@@ -1368,18 +1372,18 @@
         <v>12</v>
       </c>
       <c r="D22" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E22" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F22" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B23" t="s">
         <v>7</v>
@@ -1388,18 +1392,18 @@
         <v>8</v>
       </c>
       <c r="D23" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E23" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F23" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>7</v>
@@ -1414,12 +1418,12 @@
         <v>37</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B25" t="s">
         <v>7</v>
@@ -1428,58 +1432,58 @@
         <v>12</v>
       </c>
       <c r="D25" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E25" t="s">
         <v>13</v>
       </c>
       <c r="F25" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
+        <v>75</v>
+      </c>
+      <c r="B26" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" t="s">
+        <v>76</v>
+      </c>
+      <c r="E26" t="s">
         <v>77</v>
       </c>
-      <c r="B26" t="s">
-        <v>61</v>
-      </c>
-      <c r="C26" t="s">
-        <v>8</v>
-      </c>
-      <c r="D26" t="s">
-        <v>78</v>
-      </c>
-      <c r="E26" t="s">
-        <v>79</v>
-      </c>
       <c r="F26" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B28" t="s">
         <v>25</v>
@@ -1488,18 +1492,18 @@
         <v>8</v>
       </c>
       <c r="D28" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E28" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F28" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B29" t="s">
         <v>25</v>
@@ -1511,15 +1515,15 @@
         <v>33</v>
       </c>
       <c r="E29" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F29" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>25</v>
@@ -1528,18 +1532,18 @@
         <v>8</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B31" t="s">
         <v>7</v>
@@ -1554,15 +1558,15 @@
         <v>42</v>
       </c>
       <c r="F31" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B32" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C32" t="s">
         <v>12</v>
@@ -1574,12 +1578,12 @@
         <v>42</v>
       </c>
       <c r="F32" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
-        <v>92</v>
+        <v>180</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>7</v>
@@ -1588,18 +1592,18 @@
         <v>8</v>
       </c>
       <c r="D33" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E33" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E33" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="F33" s="1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>31</v>
@@ -1608,38 +1612,38 @@
         <v>12</v>
       </c>
       <c r="D34" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E34" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E34" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="F34" s="1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
-        <v>94</v>
+        <v>181</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>31</v>
@@ -1651,15 +1655,15 @@
         <v>16</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>25</v>
@@ -1668,18 +1672,18 @@
         <v>8</v>
       </c>
       <c r="D37" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E37" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E37" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="F37" s="1" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>25</v>
@@ -1688,18 +1692,18 @@
         <v>8</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>25</v>
@@ -1708,18 +1712,18 @@
         <v>8</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>25</v>
@@ -1728,18 +1732,18 @@
         <v>8</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>25</v>
@@ -1748,18 +1752,18 @@
         <v>8</v>
       </c>
       <c r="D41" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E41" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E41" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="F41" s="1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A42" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>25</v>
@@ -1768,38 +1772,38 @@
         <v>12</v>
       </c>
       <c r="D42" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E42" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E42" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="F42" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B43" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C43" t="s">
         <v>8</v>
       </c>
       <c r="D43" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E43" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="F43" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B44" t="s">
         <v>7</v>
@@ -1808,101 +1812,101 @@
         <v>8</v>
       </c>
       <c r="D44" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E44" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="F44" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B45" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C45" t="s">
         <v>12</v>
       </c>
       <c r="D45" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E45" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="F45" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B46" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C46" t="s">
         <v>8</v>
       </c>
       <c r="D46" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E46" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="F46" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B47" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C47" t="s">
         <v>8</v>
       </c>
       <c r="D47" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E47" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F47" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B48" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C48" t="s">
         <v>8</v>
       </c>
       <c r="D48" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E48" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="F48" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B49" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C49" t="s">
         <v>8</v>
@@ -1911,15 +1915,15 @@
         <v>22</v>
       </c>
       <c r="E49" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="F49" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B50" t="s">
         <v>25</v>
@@ -1928,18 +1932,18 @@
         <v>8</v>
       </c>
       <c r="D50" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E50" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="F50" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A51" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>25</v>
@@ -1948,18 +1952,18 @@
         <v>8</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A52" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B52" t="s">
         <v>25</v>
@@ -1968,13 +1972,13 @@
         <v>8</v>
       </c>
       <c r="D52" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E52" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="F52" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>

</xml_diff>